<commit_message>
First commit to new repo
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/Data.xlsx
+++ b/src/test/resources/xls/Data.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="13995" windowHeight="7005" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="admin" sheetId="4" r:id="rId2"/>
     <sheet name="TestCases" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:D21"/>
 </workbook>
 </file>
 
@@ -557,7 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -872,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>